<commit_message>
links na logo, padding no fale conosco
</commit_message>
<xml_diff>
--- a/Documentação/PLANILHA DE RISCO DATAFOUND.xlsx
+++ b/Documentação/PLANILHA DE RISCO DATAFOUND.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTOS\SPTech\PROJETO\GITHUB\DATAFOUND2\DATAFOUND\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6153201-19A6-45D9-8C01-648C61430B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D417E1D-8C23-47A2-81DE-B0CB84311E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1FAAE462-2AE6-4A89-8525-C4D2B073EFEB}"/>
   </bookViews>
@@ -100,10 +100,6 @@
 do fôlego</t>
   </si>
   <si>
-    <t>Replanejamento da instalação física dos sensores em
-pontos estratégicos</t>
-  </si>
-  <si>
     <t>Mudança na estrutura física da loja cliente, 
 como dividir setores préviamente definidos</t>
   </si>
@@ -129,6 +125,9 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Replanejamento da instalação física dos sensores em pontos estratégicos</t>
   </si>
 </sst>
 </file>
@@ -152,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +176,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -270,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,6 +345,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81564BC3-9F50-45B9-9A0C-DB5DCA29BF28}">
   <dimension ref="C2:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +704,7 @@
     <row r="10" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="3:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>0</v>
@@ -709,7 +738,7 @@
       <c r="F12" s="9">
         <v>3</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="20">
         <v>9</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -732,7 +761,7 @@
       <c r="F13" s="13">
         <v>1</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="22">
         <v>1</v>
       </c>
       <c r="H13" s="13" t="s">
@@ -755,7 +784,7 @@
       <c r="F14" s="9">
         <v>1</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="22">
         <v>1</v>
       </c>
       <c r="H14" s="9" t="s">
@@ -778,7 +807,7 @@
       <c r="F15" s="13">
         <v>3</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="21">
         <v>3</v>
       </c>
       <c r="H15" s="13" t="s">
@@ -788,12 +817,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="3:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="8">
         <v>5</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="9">
         <v>2</v>
@@ -801,14 +830,14 @@
       <c r="F16" s="9">
         <v>3</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="20">
         <v>6</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="3:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -816,7 +845,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E17" s="13">
         <v>1</v>
@@ -824,14 +853,14 @@
       <c r="F17" s="13">
         <v>1</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="22">
         <v>1</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>9</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="3:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -839,7 +868,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="9">
         <v>1</v>
@@ -847,14 +876,14 @@
       <c r="F18" s="9">
         <v>2</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="22">
         <v>2</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="3:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -862,7 +891,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="18">
         <v>1</v>
@@ -870,14 +899,14 @@
       <c r="F19" s="18">
         <v>1</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="23">
         <v>1</v>
       </c>
       <c r="H19" s="18" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="3:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>